<commit_message>
Updated the comment resolution document.
</commit_message>
<xml_diff>
--- a/homogeneous-snpsp-comment-resolution.xlsx
+++ b/homogeneous-snpsp-comment-resolution.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="36">
   <si>
     <t xml:space="preserve">No</t>
   </si>
@@ -74,19 +74,31 @@
     -- original subsections 4.2 and 4.3 form the new section 4 to discuss the universality of HSNPSP systems.</t>
   </si>
   <si>
+    <t xml:space="preserve">Reorganized the sections as suggested.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bibliography</t>
   </si>
   <si>
     <t xml:space="preserve">The reference is a bit old and should be updated by the reference for the last three years, including the papers in JMEC.</t>
   </si>
   <si>
+    <t xml:space="preserve">Added additional references. Cited 3 papers from JMEC. Additional background paragraphs are added to Section 1 and the references added are cited in those paragraphs.</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reviewer #3</t>
   </si>
   <si>
     <t xml:space="preserve">In order to make the manuscript more compact, the authors can give a comparative study of homogeneous and non-homogeneous SNPS systems. More specifically, a study regarding the number of neurons required to obtain the computational universality in the framework of homogeneous and non-homogeneous system should be mentioned. </t>
   </si>
   <si>
+    <t xml:space="preserve">Added additional discussion paragraphs in Section 5 that discuss number of neurons in homogeneous and non-homogeneous systems.</t>
+  </si>
+  <si>
     <t xml:space="preserve">There is a problem that the number of references is too small. The standard of this journal is above 30, which is very important to indicate the significance and necessity of this work. Moreover, several papers published in this journal is also important to be references. For example, in Introduction section, some representative applications on spiking neural P systems should be mentioned and the corresponding publications should be cited.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Added additional references. Additional background paragraphs are added to Section 1 and the references added are cited in those paragraphs.</t>
   </si>
   <si>
     <t xml:space="preserve">Page 8
@@ -96,7 +108,23 @@
     <t xml:space="preserve">`` can be the same. i.e. In a system $\Pi$'' --$&gt;$  i.e. </t>
   </si>
   <si>
-    <t xml:space="preserve">?????</t>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Rephrased the line </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">`` can be the same. i.e. In a system $\Pi$''.</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Page 10
@@ -111,6 +139,7 @@
         <sz val="10"/>
         <rFont val="CMU Serif"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">In the situation described in the paragraph, neurons $l_{i,3}$ and $l_{i,4}$ will have z+1 and will use Rule 5: $a^{z+1}/a → a$ while neurons $l_{i,5}$ and $l_{i,6}$ will have z+2 spikes and will use Rule 6: $a^{z+2}/a^2 → λ$. Only neurons $l_{i,3}$, $l_{i,4}$, and $r’$ will send a spike to neuron $r$ which means only 3 spikes (and not 5 spikes) will  be sent to neuron $r$ incrementing the number stored in register </t>
     </r>
@@ -120,6 +149,7 @@
         <sz val="10"/>
         <rFont val="CMU Serif"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">r</t>
     </r>
@@ -128,6 +158,7 @@
         <sz val="10"/>
         <rFont val="CMU Serif"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">. 
 </t>
@@ -147,6 +178,7 @@
         <sz val="10"/>
         <rFont val="CMU Serif"/>
         <family val="1"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Corrected the typograhic error in the paragraph. Changed ‘Rule 5’ to ‘Rule 6’. (Rule used by neurons  $l_{i,5}$ and $l_{i,6}$). The original paragraph incorrectly labels the rule as ‘Rule 5’ instead of ‘Rule 6’.</t>
     </r>
@@ -175,11 +207,12 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Nimbus Sans"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -211,14 +244,21 @@
     </font>
     <font>
       <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <name val="CMU Serif"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
     <font>
       <i val="true"/>
       <sz val="10"/>
       <name val="CMU Serif"/>
       <family val="1"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="5">
@@ -329,7 +369,7 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -420,15 +460,15 @@
   </sheetPr>
   <dimension ref="B2:F32"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="160" zoomScaleNormal="160" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E8" activeCellId="0" sqref="E8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="2.08"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="3.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="13.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="13.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="14.81"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="92.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="89.93"/>
@@ -517,9 +557,11 @@
       <c r="E6" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="F6" s="7"/>
-    </row>
-    <row r="7" customFormat="false" ht="38.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F6" s="7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="45.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B7" s="4" t="n">
         <v>5</v>
       </c>
@@ -527,58 +569,64 @@
         <v>9</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="F7" s="7"/>
+        <v>18</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="67.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B8" s="4" t="n">
         <v>6</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D8" s="4" t="s">
         <v>6</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="F8" s="7"/>
+        <v>21</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="71.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B9" s="4" t="n">
         <v>7</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="F9" s="7"/>
+        <v>23</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B10" s="4" t="n">
         <v>8</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="F10" s="7" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="121.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -586,16 +634,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="F11" s="10" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="29.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -603,16 +651,16 @@
         <v>10</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>28</v>
+        <v>32</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>29</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="42.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -620,16 +668,16 @@
         <v>11</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="D13" s="4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>30</v>
+        <v>34</v>
       </c>
       <c r="F13" s="7" t="s">
-        <v>31</v>
+        <v>35</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>